<commit_message>
Update: Newets WSDOC version
</commit_message>
<xml_diff>
--- a/dah_export_v1_0_0.xlsx
+++ b/dah_export_v1_0_0.xlsx
@@ -435,10 +435,10 @@
   <cols>
     <col width="14" customWidth="1" min="1" max="1"/>
     <col width="26" customWidth="1" min="2" max="2"/>
-    <col width="62" customWidth="1" min="3" max="3"/>
+    <col width="44" customWidth="1" min="3" max="3"/>
     <col width="14" customWidth="1" min="4" max="4"/>
-    <col width="6" customWidth="1" min="5" max="5"/>
-    <col width="70" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="5" max="5"/>
+    <col width="50" customWidth="1" min="6" max="6"/>
     <col width="70" customWidth="1" min="7" max="7"/>
     <col width="11" customWidth="1" min="8" max="8"/>
   </cols>
@@ -493,19 +493,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Triage</t>
+          <t>SystolicBloodPressure</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Første Triage kategorisering.</t>
+          <t>Blodtryksmåling (systolisk).</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="D3" t="inlineStr">
         <is>
-          <t>ResultCode</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -513,14 +513,9 @@
           <t>str</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>R = Red, O = Orange, Y = Yellow, G = Green, B = Blue</t>
-        </is>
-      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | r | o | y | g | b | </t>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -532,17 +527,17 @@
     <row r="4">
       <c r="D4" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>Integer</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+          <t>Greater than or equal to: 0</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -571,17 +566,17 @@
     <row r="6">
       <c r="D6" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>ResultCode</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>str, Enum</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+          <t xml:space="preserve">Enums/Udfald: | "y" | "n" | </t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -593,7 +588,7 @@
     <row r="7">
       <c r="D7" t="inlineStr">
         <is>
-          <t>ResultCode</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -601,14 +596,9 @@
           <t>str</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Y = Yes, N = No</t>
-        </is>
-      </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | y | n | </t>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -625,34 +615,29 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Temperature</t>
+          <t>AVPUScale</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Første temperatur måling.</t>
+          <t>Første AVPU skala</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="D9" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>ResultCode</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>float</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Enhed = grader</t>
+          <t>str, Enum</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0</t>
+          <t xml:space="preserve">Enums/Udfald: | "a" | "v" | "p" | "u" | </t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -691,29 +676,29 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SystolicBloodPressure</t>
+          <t>Triage</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Blodtryksmåling (systolisk).</t>
+          <t>Første Triage kategorisering.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="D12" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>ResultCode</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>str, Enum</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0</t>
+          <t xml:space="preserve">Enums/Udfald: | "r" | "o" | "y" | "g" | "b" | </t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -752,29 +737,29 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>GlasgowComaScale</t>
+          <t>RespiratoryRate</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Første Glasgow Coma Scale måling.</t>
+          <t>Første respirationsfrekvens måling.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="D15" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>str</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 3 | Less than or equal to: 15</t>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -786,17 +771,17 @@
     <row r="16">
       <c r="D16" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>Integer</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+          <t>Greater than or equal to: 0</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -813,29 +798,29 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>RespiratoryRate</t>
+          <t>Temperature</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Første respirationsfrekvens måling.</t>
+          <t>Første temperatur måling.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="D18" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>str</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0</t>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -847,17 +832,22 @@
     <row r="19">
       <c r="D19" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>Float</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Enhed = grader</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+          <t>Greater than or equal to: 0</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -874,19 +864,19 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>PainEvaluation</t>
+          <t>GlasgowComaScale</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Første smertemåling.</t>
+          <t>Første Glasgow Coma Scale måling.</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="D21" t="inlineStr">
         <is>
-          <t>ResultCode</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -894,14 +884,9 @@
           <t>str</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Hvis der angives 'Andet' i type, er det muligt at indsende yderligere information i 'Note' element.</t>
-        </is>
-      </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | vas | nrs | vrs | andet | </t>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -913,44 +898,39 @@
     <row r="22">
       <c r="D22" t="inlineStr">
         <is>
-          <t>Note</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>str</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Bruges ved 'andet' type af smertescore</t>
+          <t>Integer</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Greater than or equal to: 3 | Less than or equal to: 15</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>ResultValue</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>float</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Værdi for 'smertescore</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Greater than or equal to: 0</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>True</t>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>PulseRate</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Første pulsmåling.</t>
         </is>
       </c>
     </row>
@@ -977,124 +957,129 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>ResultValue</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Integer</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Greater than or equal to: 0</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
         <is>
           <t>Observation</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="B26" t="inlineStr">
         <is>
           <t>OxygenSaturation</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>Første iltmætningsmåling.</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>DateTime</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>str</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>True</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="D27" t="inlineStr">
         <is>
+          <t>DateTime</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>str</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="D28" t="inlineStr">
+        <is>
           <t>ResultValue</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>float</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Float</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
         <is>
           <t>Enhed = %</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="G28" t="inlineStr">
         <is>
           <t>Greater than or equal to: 0 | Less than or equal to: 100</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
         <is>
           <t>Observation</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>PulseRate</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Første pulsmåling.</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>DateTime</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>str</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>True</t>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>PainEvaluation</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Første smertemåling.</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>ResultCode</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>int</t>
+          <t>str, Enum</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Se webservice dokumentation.</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0</t>
+          <t xml:space="preserve">Enums/Udfald: | "vas" | "nrs" | "vrs" | "andet" | </t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1104,41 +1089,46 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>AVPUScale</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Første AVPU skala (bevidsthed).</t>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>DateTime</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>str</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
         <is>
-          <t>ResultCode</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>Float</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>A = Alert, V = Verbal, P = Pain, U = Unresponsive</t>
+          <t>Værdi for smertescore</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | a | v | p | u | </t>
+          <t>Greater than or equal to: 0</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1150,22 +1140,17 @@
     <row r="33">
       <c r="D33" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>Note</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>str</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>True</t>
+          <t>String</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Bruges ved 'andet' type af smertescore</t>
         </is>
       </c>
     </row>
@@ -1182,7 +1167,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Dato for første afsluttet lægenotat samt notattype</t>
+          <t>Første afsluttet lægenotat</t>
         </is>
       </c>
     </row>
@@ -1197,6 +1182,11 @@
           <t>str</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Dato for første afsluttet lægenotat</t>
+        </is>
+      </c>
       <c r="G35" t="inlineStr">
         <is>
           <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
@@ -1216,7 +1206,12 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>String</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Notattype for første afsluttet lægenotat</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">

</xml_diff>

<commit_message>
updating json + url
</commit_message>
<xml_diff>
--- a/dah_export_v1_0_0.xlsx
+++ b/dah_export_v1_0_0.xlsx
@@ -493,12 +493,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SystolicBloodPressure</t>
+          <t>RespiratoryRate</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Blodtryksmåling (systolisk).</t>
+          <t>Første respirationsfrekvens måling.</t>
         </is>
       </c>
     </row>
@@ -554,12 +554,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>OxygenDemand</t>
+          <t>AVPUScale</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Første iltbehov.</t>
+          <t>Første AVPU skala</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "y" | "n" | </t>
+          <t xml:space="preserve">Enums/Udfald: | "a" | "v" | "p" | "u" | </t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -615,29 +615,29 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>AVPUScale</t>
+          <t>PulseRate</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Første AVPU skala</t>
+          <t>Første pulsmåling.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="D9" t="inlineStr">
         <is>
-          <t>ResultCode</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>str, Enum</t>
+          <t>str</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "a" | "v" | "p" | "u" | </t>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -649,17 +649,17 @@
     <row r="10">
       <c r="D10" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>Integer</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+          <t>Greater than or equal to: 0</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -676,12 +676,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Triage</t>
+          <t>OxygenDemand</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Første Triage kategorisering.</t>
+          <t>Første iltbehov.</t>
         </is>
       </c>
     </row>
@@ -698,7 +698,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t xml:space="preserve">Enums/Udfald: | "r" | "o" | "y" | "g" | "b" | </t>
+          <t xml:space="preserve">Enums/Udfald: | "y" | "n" | </t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -737,12 +737,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>RespiratoryRate</t>
+          <t>OxygenSaturation</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Første respirationsfrekvens måling.</t>
+          <t>Første iltmætningsmåling.</t>
         </is>
       </c>
     </row>
@@ -776,12 +776,17 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Integer</t>
+          <t>Float</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Enhed = %</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0</t>
+          <t>Greater than or equal to: 0 | Less than or equal to: 100</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -798,29 +803,29 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Temperature</t>
+          <t>Triage</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Første temperatur måling.</t>
+          <t>Første Triage kategorisering.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="D18" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>ResultCode</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>str, Enum</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+          <t xml:space="preserve">Enums/Udfald: | "r" | "o" | "y" | "g" | "b" | </t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -832,22 +837,17 @@
     <row r="19">
       <c r="D19" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Float</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Enhed = grader</t>
+          <t>str</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0</t>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -925,12 +925,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>PulseRate</t>
+          <t>Temperature</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Første pulsmåling.</t>
+          <t>Første temperatur måling.</t>
         </is>
       </c>
     </row>
@@ -964,7 +964,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Integer</t>
+          <t>Float</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Enhed = grader</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -986,29 +991,34 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>OxygenSaturation</t>
+          <t>PainEvaluation</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Første iltmætningsmåling.</t>
+          <t>Første smertemåling.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="D27" t="inlineStr">
         <is>
-          <t>DateTime</t>
+          <t>ResultCode</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>str</t>
+          <t>str, Enum</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Se webservice dokumentation.</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+          <t xml:space="preserve">Enums/Udfald: | "vas" | "nrs" | "vrs" | "andet" | </t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1020,115 +1030,100 @@
     <row r="28">
       <c r="D28" t="inlineStr">
         <is>
+          <t>DateTime</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>str</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="D29" t="inlineStr">
+        <is>
           <t>ResultValue</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>Float</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Enhed = %</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>Greater than or equal to: 0 | Less than or equal to: 100</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Observation</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>PainEvaluation</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Første smertemåling.</t>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Værdi for smertescore</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Greater than or equal to: 0</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="D30" t="inlineStr">
         <is>
-          <t>ResultCode</t>
+          <t>Note</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>str, Enum</t>
+          <t>String</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Se webservice dokumentation.</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Enums/Udfald: | "vas" | "nrs" | "vrs" | "andet" | </t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>True</t>
+          <t>Bruges ved 'andet' type af smertescore</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>DateTime</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>str</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>True</t>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Observation</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>SystolicBloodPressure</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Blodtryksmåling (systolisk).</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="inlineStr">
         <is>
-          <t>ResultValue</t>
+          <t>DateTime</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Float</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Værdi for smertescore</t>
+          <t>str</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Greater than or equal to: 0</t>
+          <t>Date format: | DD-MM-YYYY HH:MM:SS |</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -1140,17 +1135,22 @@
     <row r="33">
       <c r="D33" t="inlineStr">
         <is>
-          <t>Note</t>
+          <t>ResultValue</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>String</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>Bruges ved 'andet' type af smertescore</t>
+          <t>Integer</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Greater than or equal to: 0</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>True</t>
         </is>
       </c>
     </row>

</xml_diff>